<commit_message>
archivo de pruebas actualizado
</commit_message>
<xml_diff>
--- a/tbc/Pruebas Escalabilidad/Pruebas.xlsx
+++ b/tbc/Pruebas Escalabilidad/Pruebas.xlsx
@@ -5,22 +5,22 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\CODD.sis.virtual.uniandes.edu.co\Estudiantes\Profiles\js.ruiz127\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Santiago\Desktop\Universidad\Arquisoft\experimento\tbc\Pruebas Escalabilidad\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja3" sheetId="3" r:id="rId1"/>
     <sheet name="Hoja1" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="39">
   <si>
     <t>Repetición</t>
   </si>
@@ -89,6 +89,54 @@
   </si>
   <si>
     <t>3,4/sec</t>
+  </si>
+  <si>
+    <t>GET_Vcubs</t>
+  </si>
+  <si>
+    <t>Iteración anterior</t>
+  </si>
+  <si>
+    <t>Nueva Iteración</t>
+  </si>
+  <si>
+    <t>18,9/sec</t>
+  </si>
+  <si>
+    <t>62,5/sec</t>
+  </si>
+  <si>
+    <t>70,4/sec</t>
+  </si>
+  <si>
+    <t>65,4/sec</t>
+  </si>
+  <si>
+    <t>64,1/sec</t>
+  </si>
+  <si>
+    <t>65,6/sec</t>
+  </si>
+  <si>
+    <t>56,7/sec</t>
+  </si>
+  <si>
+    <t>47,0/sec</t>
+  </si>
+  <si>
+    <t>POST_Vcub</t>
+  </si>
+  <si>
+    <t>34,0/sec</t>
+  </si>
+  <si>
+    <t>36,4/sec</t>
+  </si>
+  <si>
+    <t>25,0/sec</t>
+  </si>
+  <si>
+    <t>21,6/sec</t>
   </si>
 </sst>
 </file>
@@ -351,7 +399,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -376,9 +424,6 @@
     <xf numFmtId="9" fontId="3" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="3" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="3" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -391,6 +436,12 @@
     <xf numFmtId="9" fontId="3" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="3" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -700,11 +751,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="996262560"/>
-        <c:axId val="996263104"/>
+        <c:axId val="148470240"/>
+        <c:axId val="148547576"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="996262560"/>
+        <c:axId val="148470240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -733,12 +784,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="996263104"/>
+        <c:crossAx val="148547576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="996263104"/>
+        <c:axId val="148547576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -768,7 +819,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="996262560"/>
+        <c:crossAx val="148470240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1052,11 +1103,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="991902768"/>
-        <c:axId val="991897328"/>
+        <c:axId val="148390776"/>
+        <c:axId val="148391160"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="991902768"/>
+        <c:axId val="148390776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1085,12 +1136,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="991897328"/>
+        <c:crossAx val="148391160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="991897328"/>
+        <c:axId val="148391160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1120,7 +1171,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="991902768"/>
+        <c:crossAx val="148390776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1503,17 +1554,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A5:L45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="K40" sqref="K40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="5" spans="2:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="24"/>
+      <c r="C5" s="36"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -1636,7 +1687,7 @@
       <c r="L12" s="2"/>
     </row>
     <row r="13" spans="2:12" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="35">
+      <c r="B13" s="34">
         <v>6</v>
       </c>
       <c r="C13" s="12">
@@ -1648,7 +1699,7 @@
       <c r="E13" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="F13" s="36">
+      <c r="F13" s="35">
         <v>0.20749999999999999</v>
       </c>
     </row>
@@ -1667,14 +1718,14 @@
       <c r="E16" s="3"/>
       <c r="F16" s="5"/>
     </row>
-    <row r="17" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
@@ -1682,7 +1733,7 @@
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
@@ -1690,17 +1741,17 @@
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="2:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B20" s="24" t="s">
+    <row r="20" spans="2:12" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B20" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="24"/>
+      <c r="C20" s="36"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
     </row>
-    <row r="21" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -1708,7 +1759,7 @@
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B22" s="14" t="s">
         <v>0</v>
       </c>
@@ -1726,7 +1777,7 @@
       </c>
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B23" s="17">
         <v>1</v>
       </c>
@@ -1744,7 +1795,7 @@
       </c>
       <c r="G23" s="2"/>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B24" s="17">
         <v>2</v>
       </c>
@@ -1762,7 +1813,7 @@
       </c>
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B25" s="17">
         <v>3</v>
       </c>
@@ -1780,7 +1831,7 @@
       </c>
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B26" s="17">
         <v>4</v>
       </c>
@@ -1798,7 +1849,7 @@
       </c>
       <c r="G26" s="2"/>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B27" s="17">
         <v>5</v>
       </c>
@@ -1816,50 +1867,50 @@
       </c>
       <c r="G27" s="2"/>
     </row>
-    <row r="28" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="25">
+    <row r="28" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="24">
         <v>6</v>
       </c>
-      <c r="C28" s="27">
+      <c r="C28" s="26">
         <v>400</v>
       </c>
-      <c r="D28" s="27">
+      <c r="D28" s="26">
         <v>35200</v>
       </c>
-      <c r="E28" s="27" t="s">
+      <c r="E28" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="F28" s="28">
+      <c r="F28" s="27">
         <v>0</v>
       </c>
       <c r="G28" s="2"/>
     </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="32">
+    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B29" s="31">
         <v>7</v>
       </c>
-      <c r="C29" s="33">
+      <c r="C29" s="32">
         <v>500</v>
       </c>
-      <c r="D29" s="33">
+      <c r="D29" s="32">
         <v>44977</v>
       </c>
-      <c r="E29" s="33" t="s">
+      <c r="E29" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="F29" s="34">
+      <c r="F29" s="33">
         <v>3.4000000000000002E-2</v>
       </c>
       <c r="G29" s="2"/>
     </row>
-    <row r="30" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B30" s="4"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
       <c r="F30" s="5"/>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B31" s="4"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
@@ -1867,22 +1918,36 @@
       <c r="F31" s="5"/>
       <c r="G31" s="2"/>
     </row>
-    <row r="32" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="4"/>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
       <c r="F32" s="5"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H32" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="I32" s="37"/>
+      <c r="J32" s="37"/>
+      <c r="K32" s="37"/>
+      <c r="L32" s="37"/>
+    </row>
+    <row r="33" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B33" s="4"/>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
       <c r="F33" s="5"/>
       <c r="G33" s="2"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H33" s="36" t="s">
+        <v>5</v>
+      </c>
+      <c r="I33" s="36"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="2"/>
+      <c r="L33" s="2"/>
+    </row>
+    <row r="34" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -1892,8 +1957,11 @@
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -1901,10 +1969,23 @@
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
-      <c r="I35" s="2"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H35" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="I35" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="J35" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="K35" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="L35" s="16" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -1912,10 +1993,23 @@
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H36" s="17">
+        <v>1</v>
+      </c>
+      <c r="I36" s="6">
+        <v>5</v>
+      </c>
+      <c r="J36" s="6">
+        <v>48</v>
+      </c>
+      <c r="K36" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="L36" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -1923,10 +2017,23 @@
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
-      <c r="H37" s="2"/>
-      <c r="I37" s="2"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H37" s="17">
+        <v>2</v>
+      </c>
+      <c r="I37" s="6">
+        <v>30</v>
+      </c>
+      <c r="J37" s="6">
+        <v>191</v>
+      </c>
+      <c r="K37" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="L37" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -1934,10 +2041,23 @@
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
-      <c r="H38" s="2"/>
-      <c r="I38" s="2"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H38" s="17">
+        <v>3</v>
+      </c>
+      <c r="I38" s="6">
+        <v>50</v>
+      </c>
+      <c r="J38" s="6">
+        <v>352</v>
+      </c>
+      <c r="K38" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="L38" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -1945,10 +2065,23 @@
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
-      <c r="H39" s="2"/>
-      <c r="I39" s="2"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H39" s="17">
+        <v>4</v>
+      </c>
+      <c r="I39" s="6">
+        <v>80</v>
+      </c>
+      <c r="J39" s="6">
+        <v>589</v>
+      </c>
+      <c r="K39" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="L39" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -1956,10 +2089,23 @@
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
-      <c r="H40" s="2"/>
-      <c r="I40" s="2"/>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H40" s="17">
+        <v>5</v>
+      </c>
+      <c r="I40" s="6">
+        <v>200</v>
+      </c>
+      <c r="J40" s="6">
+        <v>1366</v>
+      </c>
+      <c r="K40" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="L40" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -1967,10 +2113,23 @@
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
-      <c r="H41" s="2"/>
-      <c r="I41" s="2"/>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H41" s="34">
+        <v>6</v>
+      </c>
+      <c r="I41" s="12">
+        <v>400</v>
+      </c>
+      <c r="J41" s="12">
+        <v>46017</v>
+      </c>
+      <c r="K41" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="L41" s="35">
+        <v>0.20749999999999999</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -1981,7 +2140,7 @@
       <c r="H42" s="2"/>
       <c r="I42" s="2"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -1992,7 +2151,7 @@
       <c r="H43" s="2"/>
       <c r="I43" s="2"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -2003,7 +2162,7 @@
       <c r="H44" s="2"/>
       <c r="I44" s="2"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -2015,9 +2174,11 @@
       <c r="I45" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B20:C20"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="H32:L32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2026,10 +2187,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:H35"/>
+  <dimension ref="A1:M35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" topLeftCell="E4" workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2042,23 +2203,57 @@
     <col min="12" max="13" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B3" s="24" t="s">
+    <row r="1" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="I1" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
+    </row>
+    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B2" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="I2" t="e">
+        <f>+I1:K2I1:M2I1:L2I1:I1:M2</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="3" spans="2:13" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B3" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="24"/>
+      <c r="C3" s="36"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I3" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="36"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+    </row>
+    <row r="4" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B5" s="7" t="s">
         <v>0</v>
       </c>
@@ -2074,8 +2269,23 @@
       <c r="F5" s="9" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I5" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="L5" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="M5" s="9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B6" s="10">
         <v>1</v>
       </c>
@@ -2091,8 +2301,23 @@
       <c r="F6" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I6" s="10">
+        <v>1</v>
+      </c>
+      <c r="J6" s="6">
+        <v>50</v>
+      </c>
+      <c r="K6" s="6">
+        <v>253</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="M6" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" s="10">
         <v>2</v>
       </c>
@@ -2108,8 +2333,23 @@
       <c r="F7" s="22">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I7" s="10">
+        <v>2</v>
+      </c>
+      <c r="J7" s="6">
+        <v>500</v>
+      </c>
+      <c r="K7" s="6">
+        <v>3960</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="M7" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B8" s="10">
         <v>3</v>
       </c>
@@ -2125,48 +2365,90 @@
       <c r="F8" s="21">
         <v>0.63200000000000001</v>
       </c>
-    </row>
-    <row r="9" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="29">
+      <c r="I8" s="10">
+        <v>3</v>
+      </c>
+      <c r="J8" s="6">
+        <v>1000</v>
+      </c>
+      <c r="K8" s="6">
+        <v>10014</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="M8" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="28">
         <v>4</v>
       </c>
-      <c r="C9" s="27">
+      <c r="C9" s="26">
         <v>4000</v>
       </c>
-      <c r="D9" s="27">
+      <c r="D9" s="26">
         <v>205870</v>
       </c>
-      <c r="E9" s="27" t="s">
+      <c r="E9" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="30">
+      <c r="F9" s="29">
         <v>0.42680000000000001</v>
       </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I9" s="28">
+        <v>4</v>
+      </c>
+      <c r="J9" s="26">
+        <v>4000</v>
+      </c>
+      <c r="K9" s="26">
+        <v>41918</v>
+      </c>
+      <c r="L9" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="M9" s="29">
+        <v>0.22919999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="5"/>
     </row>
-    <row r="13" spans="2:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B13" s="24" t="s">
+    <row r="13" spans="2:13" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B13" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="24"/>
+      <c r="C13" s="36"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I13" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="J13" s="36"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+    </row>
+    <row r="14" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B15" s="14" t="s">
         <v>0</v>
       </c>
@@ -2182,8 +2464,23 @@
       <c r="F15" s="16" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="I15" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="J15" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="K15" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="L15" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="M15" s="16" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B16" s="17">
         <v>1</v>
       </c>
@@ -2199,8 +2496,23 @@
       <c r="F16" s="18">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I16" s="17">
+        <v>1</v>
+      </c>
+      <c r="J16" s="20">
+        <v>50</v>
+      </c>
+      <c r="K16" s="13">
+        <v>827</v>
+      </c>
+      <c r="L16" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="M16" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B17" s="17">
         <v>2</v>
       </c>
@@ -2216,8 +2528,23 @@
       <c r="F17" s="23">
         <v>0.28199999999999997</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I17" s="17">
+        <v>2</v>
+      </c>
+      <c r="J17" s="20">
+        <v>500</v>
+      </c>
+      <c r="K17" s="13">
+        <v>6548</v>
+      </c>
+      <c r="L17" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="M17" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B18" s="17">
         <v>3</v>
       </c>
@@ -2233,25 +2560,55 @@
       <c r="F18" s="22">
         <v>0.36599999999999999</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="25">
+      <c r="I18" s="17">
+        <v>3</v>
+      </c>
+      <c r="J18" s="20">
+        <v>1000</v>
+      </c>
+      <c r="K18" s="13">
+        <v>17994</v>
+      </c>
+      <c r="L18" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="M18" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="24">
         <v>4</v>
       </c>
-      <c r="C19" s="26">
+      <c r="C19" s="25">
         <v>4000</v>
       </c>
-      <c r="D19" s="27">
+      <c r="D19" s="26">
         <v>307650</v>
       </c>
-      <c r="E19" s="27" t="s">
+      <c r="E19" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="F19" s="31">
+      <c r="F19" s="30">
         <v>0.40400000000000003</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I19" s="24">
+        <v>4</v>
+      </c>
+      <c r="J19" s="25">
+        <v>4000</v>
+      </c>
+      <c r="K19" s="26">
+        <v>61630</v>
+      </c>
+      <c r="L19" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="M19" s="30">
+        <v>0.34849999999999998</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
@@ -2259,42 +2616,42 @@
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B21" s="4"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
       <c r="F21" s="5"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B22" s="4"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="5"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B23" s="4"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="5"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B24" s="4"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="5"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B25" s="4"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="5"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
@@ -2302,7 +2659,7 @@
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -2312,7 +2669,7 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -2322,7 +2679,7 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -2332,7 +2689,7 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -2342,7 +2699,7 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -2383,9 +2740,13 @@
       <c r="H35" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="6">
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B13:C13"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="I1:M1"/>
+    <mergeCell ref="I13:J13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Acualización de informe de pruebas.
</commit_message>
<xml_diff>
--- a/tbc/Pruebas Escalabilidad/Pruebas.xlsx
+++ b/tbc/Pruebas Escalabilidad/Pruebas.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Santiago\Desktop\Universidad\Arquisoft\experimento\tbc\Pruebas Escalabilidad\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wrt6000V1\RubymineProjects\ProyectoArquisoft\Grupo-06\tbc\Pruebas Escalabilidad\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="46">
   <si>
     <t>Repetición</t>
   </si>
@@ -137,6 +137,27 @@
   </si>
   <si>
     <t>21,6/sec</t>
+  </si>
+  <si>
+    <t>GET_Tranvía(Primera Prueba)</t>
+  </si>
+  <si>
+    <t>POST_Tranvía(Primera Prueba)</t>
+  </si>
+  <si>
+    <t>Aumento de rendimiento</t>
+  </si>
+  <si>
+    <t>Comparación de una solicitud http Get</t>
+  </si>
+  <si>
+    <t>Tiempo respuesta medio(ms) Primera Prueba</t>
+  </si>
+  <si>
+    <t>Tiempo respuesta medio(ms) Segunda Prueba</t>
+  </si>
+  <si>
+    <t>Comparación de una solicitud http Post</t>
   </si>
 </sst>
 </file>
@@ -213,7 +234,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -395,11 +416,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -421,7 +479,6 @@
     <xf numFmtId="9" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="3" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="3" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="3" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -429,7 +486,6 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="3" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="3" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="3" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -442,6 +498,82 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -508,7 +640,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja3!$B$5</c:f>
+              <c:f>Hoja1!$C$44</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -540,7 +672,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja3!$C$8:$C$13</c:f>
+              <c:f>Hoja1!$D$47:$D$52</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -567,7 +699,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja3!$D$8:$D$13</c:f>
+              <c:f>Hoja1!$E$47:$E$52</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -599,7 +731,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja3!$B$20</c:f>
+              <c:f>Hoja1!$C$59</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -631,7 +763,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja3!$C$23:$C$29</c:f>
+              <c:f>Hoja1!$D$62:$D$68</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -661,7 +793,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja3!$D$23:$D$29</c:f>
+              <c:f>Hoja1!$E$62:$E$68</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -751,11 +883,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="148470240"/>
-        <c:axId val="148547576"/>
+        <c:axId val="220283536"/>
+        <c:axId val="220284320"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="148470240"/>
+        <c:axId val="220283536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -784,12 +916,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="148547576"/>
+        <c:crossAx val="220284320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="148547576"/>
+        <c:axId val="220284320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -819,7 +951,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="148470240"/>
+        <c:crossAx val="220283536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -894,7 +1026,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>GET_Tranvías</c:v>
+                  <c:v>GET_Tranvía(Primera Prueba)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -973,7 +1105,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>POST_Tranvía</c:v>
+                  <c:v>POST_Tranvía(Primera Prueba)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1047,12 +1179,7 @@
           <c:idx val="1"/>
           <c:order val="2"/>
           <c:tx>
-            <c:strRef>
-              <c:f>Hoja1!$B$27</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-              </c:strCache>
-            </c:strRef>
+            <c:v>Get_Vcub(Segunda Prueba)</c:v>
           </c:tx>
           <c:spPr>
             <a:ln>
@@ -1077,19 +1204,93 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja1!$C$30:$C$33</c:f>
+              <c:f>Hoja1!$J$6:$J$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4000</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja1!$D$30:$D$33</c:f>
+              <c:f>Hoja1!$K$6:$K$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>253</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3960</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10014</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>41918</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Post_Vcub(Segunda Prueba)</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Hoja1!$J$16:$J$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Hoja1!$K$16:$K$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>827</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6548</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17994</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>61630</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1103,11 +1304,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="148390776"/>
-        <c:axId val="148391160"/>
+        <c:axId val="220284712"/>
+        <c:axId val="220285888"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="148390776"/>
+        <c:axId val="220284712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1136,12 +1337,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="148391160"/>
+        <c:crossAx val="220285888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="148391160"/>
+        <c:axId val="220285888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1171,7 +1372,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="148390776"/>
+        <c:crossAx val="220284712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1197,16 +1398,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>600076</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>523876</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1554,353 +1755,73 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A5:L45"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="K40" sqref="K40"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="5" spans="2:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B5" s="36" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="36"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
+    <row r="5" spans="7:12" x14ac:dyDescent="0.25">
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
+    <row r="6" spans="7:12" x14ac:dyDescent="0.25">
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="F7" s="16" t="s">
-        <v>1</v>
-      </c>
+    <row r="7" spans="7:12" x14ac:dyDescent="0.25">
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="17">
-        <v>1</v>
-      </c>
-      <c r="C8" s="6">
-        <v>5</v>
-      </c>
-      <c r="D8" s="6">
-        <v>524</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F8" s="18">
-        <v>0</v>
-      </c>
+    <row r="8" spans="7:12" x14ac:dyDescent="0.25">
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="17">
-        <v>2</v>
-      </c>
-      <c r="C9" s="6">
-        <v>30</v>
-      </c>
-      <c r="D9" s="6">
-        <v>3163</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" s="11">
-        <v>0</v>
-      </c>
+    <row r="9" spans="7:12" x14ac:dyDescent="0.25">
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="17">
-        <v>3</v>
-      </c>
-      <c r="C10" s="6">
-        <v>50</v>
-      </c>
-      <c r="D10" s="6">
-        <v>8537</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F10" s="11">
-        <v>0</v>
-      </c>
+    <row r="10" spans="7:12" x14ac:dyDescent="0.25">
       <c r="G10" s="2"/>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="17">
-        <v>4</v>
-      </c>
-      <c r="C11" s="6">
-        <v>80</v>
-      </c>
-      <c r="D11" s="6">
-        <v>13767</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B12" s="17">
-        <v>5</v>
-      </c>
-      <c r="C12" s="6">
-        <v>200</v>
-      </c>
-      <c r="D12" s="6">
-        <v>35355</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F12" s="11">
-        <v>0</v>
-      </c>
+    <row r="12" spans="7:12" x14ac:dyDescent="0.25">
       <c r="G12" s="2"/>
       <c r="L12" s="2"/>
     </row>
-    <row r="13" spans="2:12" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="34">
-        <v>6</v>
-      </c>
-      <c r="C13" s="12">
-        <v>400</v>
-      </c>
-      <c r="D13" s="12">
-        <v>46017</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="F13" s="35">
-        <v>0.20749999999999999</v>
-      </c>
-    </row>
-    <row r="14" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="5"/>
-    </row>
-    <row r="16" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="5"/>
-    </row>
-    <row r="17" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="5"/>
-    </row>
+    <row r="13" spans="7:12" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="7:12" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="7:12" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="7:12" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="18" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="2:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B20" s="36" t="s">
-        <v>6</v>
-      </c>
-      <c r="C20" s="36"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
       <c r="G20" s="2"/>
     </row>
-    <row r="21" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
       <c r="G21" s="2"/>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B22" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="C22" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="D22" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="E22" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="F22" s="16" t="s">
-        <v>1</v>
-      </c>
       <c r="G22" s="2"/>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B23" s="17">
-        <v>1</v>
-      </c>
-      <c r="C23" s="6">
-        <v>5</v>
-      </c>
-      <c r="D23" s="6">
-        <v>1612</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F23" s="18">
-        <v>0</v>
-      </c>
       <c r="G23" s="2"/>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B24" s="17">
-        <v>2</v>
-      </c>
-      <c r="C24" s="6">
-        <v>30</v>
-      </c>
-      <c r="D24" s="6">
-        <v>7175</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F24" s="11">
-        <v>0</v>
-      </c>
       <c r="G24" s="2"/>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B25" s="17">
-        <v>3</v>
-      </c>
-      <c r="C25" s="6">
-        <v>50</v>
-      </c>
-      <c r="D25" s="6">
-        <v>8988</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F25" s="11">
-        <v>0</v>
-      </c>
       <c r="G25" s="2"/>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B26" s="17">
-        <v>4</v>
-      </c>
-      <c r="C26" s="6">
-        <v>80</v>
-      </c>
-      <c r="D26" s="6">
-        <v>16977</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F26" s="11">
-        <v>0</v>
-      </c>
       <c r="G26" s="2"/>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B27" s="17">
-        <v>5</v>
-      </c>
-      <c r="C27" s="6">
-        <v>200</v>
-      </c>
-      <c r="D27" s="6">
-        <v>20330</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F27" s="11">
-        <v>0</v>
-      </c>
       <c r="G27" s="2"/>
     </row>
-    <row r="28" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="24">
-        <v>6</v>
-      </c>
-      <c r="C28" s="26">
-        <v>400</v>
-      </c>
-      <c r="D28" s="26">
-        <v>35200</v>
-      </c>
-      <c r="E28" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="F28" s="27">
-        <v>0</v>
-      </c>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
       <c r="G28" s="2"/>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B29" s="31">
-        <v>7</v>
-      </c>
-      <c r="C29" s="32">
-        <v>500</v>
-      </c>
-      <c r="D29" s="32">
-        <v>44977</v>
-      </c>
-      <c r="E29" s="32" t="s">
-        <v>19</v>
-      </c>
-      <c r="F29" s="33">
-        <v>3.4000000000000002E-2</v>
-      </c>
       <c r="G29" s="2"/>
     </row>
     <row r="30" spans="2:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1924,13 +1845,13 @@
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
       <c r="F32" s="5"/>
-      <c r="H32" s="37" t="s">
+      <c r="H32" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="I32" s="37"/>
-      <c r="J32" s="37"/>
-      <c r="K32" s="37"/>
-      <c r="L32" s="37"/>
+      <c r="I32" s="35"/>
+      <c r="J32" s="35"/>
+      <c r="K32" s="35"/>
+      <c r="L32" s="35"/>
     </row>
     <row r="33" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B33" s="4"/>
@@ -1939,10 +1860,10 @@
       <c r="E33" s="3"/>
       <c r="F33" s="5"/>
       <c r="G33" s="2"/>
-      <c r="H33" s="36" t="s">
+      <c r="H33" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="I33" s="36"/>
+      <c r="I33" s="34"/>
       <c r="J33" s="2"/>
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
@@ -2113,7 +2034,7 @@
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
-      <c r="H41" s="34">
+      <c r="H41" s="32">
         <v>6</v>
       </c>
       <c r="I41" s="12">
@@ -2125,7 +2046,7 @@
       <c r="K41" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="L41" s="35">
+      <c r="L41" s="33">
         <v>0.20749999999999999</v>
       </c>
     </row>
@@ -2174,9 +2095,7 @@
       <c r="I45" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B20:C20"/>
+  <mergeCells count="2">
     <mergeCell ref="H33:I33"/>
     <mergeCell ref="H32:L32"/>
   </mergeCells>
@@ -2187,10 +2106,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M35"/>
+  <dimension ref="A1:T68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E4" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+    <sheetView tabSelected="1" topLeftCell="L4" workbookViewId="0">
+      <selection activeCell="P4" sqref="P4:T19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2201,47 +2120,51 @@
     <col min="10" max="10" width="38.5703125" customWidth="1"/>
     <col min="11" max="11" width="30" customWidth="1"/>
     <col min="12" max="13" width="21.140625" customWidth="1"/>
+    <col min="16" max="16" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="23.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="I1" s="37" t="s">
+    <row r="1" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="I1" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
-    </row>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B2" s="37" t="s">
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+    </row>
+    <row r="2" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B2" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
       <c r="I2" t="e">
         <f>+I1:K2I1:M2I1:L2I1:I1:M2</f>
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="3" spans="2:13" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B3" s="36" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="36"/>
+    <row r="3" spans="2:20" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="34" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="34"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-      <c r="I3" s="36" t="s">
+      <c r="I3" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="36"/>
+      <c r="J3" s="34"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
     </row>
-    <row r="4" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -2252,21 +2175,28 @@
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
-    </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B5" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="8" t="s">
+      <c r="P4" s="45" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q4" s="46"/>
+      <c r="R4" s="46"/>
+      <c r="S4" s="46"/>
+      <c r="T4" s="47"/>
+    </row>
+    <row r="5" spans="2:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="B5" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="44" t="s">
         <v>1</v>
       </c>
       <c r="I5" s="7" t="s">
@@ -2284,21 +2214,36 @@
       <c r="M5" s="9" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B6" s="10">
+      <c r="P5" s="48" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="49" t="s">
+        <v>3</v>
+      </c>
+      <c r="R5" s="50" t="s">
+        <v>43</v>
+      </c>
+      <c r="S5" s="50" t="s">
+        <v>44</v>
+      </c>
+      <c r="T5" s="51" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B6" s="36">
         <v>1</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="37">
         <v>50</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="37">
         <v>8988</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="38">
         <v>0</v>
       </c>
       <c r="I6" s="10">
@@ -2316,21 +2261,37 @@
       <c r="M6" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B7" s="10">
+      <c r="P6" s="52">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="53">
+        <v>50</v>
+      </c>
+      <c r="R6" s="53">
+        <v>8988</v>
+      </c>
+      <c r="S6" s="53">
+        <v>253</v>
+      </c>
+      <c r="T6" s="54">
+        <f>R6/S6</f>
+        <v>35.525691699604742</v>
+      </c>
+    </row>
+    <row r="7" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B7" s="36">
         <v>2</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="37">
         <v>500</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="37">
         <v>33286</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="22">
+      <c r="F7" s="59">
         <v>0.4</v>
       </c>
       <c r="I7" s="10">
@@ -2348,21 +2309,37 @@
       <c r="M7" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B8" s="10">
+      <c r="P7" s="52">
+        <v>2</v>
+      </c>
+      <c r="Q7" s="53">
+        <v>500</v>
+      </c>
+      <c r="R7" s="53">
+        <v>33286</v>
+      </c>
+      <c r="S7" s="53">
+        <v>3960</v>
+      </c>
+      <c r="T7" s="54">
+        <f t="shared" ref="T7:T9" si="0">R7/S7</f>
+        <v>8.405555555555555</v>
+      </c>
+    </row>
+    <row r="8" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B8" s="36">
         <v>3</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="37">
         <v>1000</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="37">
         <v>25421</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="21">
+      <c r="F8" s="60">
         <v>0.63200000000000001</v>
       </c>
       <c r="I8" s="10">
@@ -2380,63 +2357,95 @@
       <c r="M8" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="28">
+      <c r="P8" s="52">
+        <v>3</v>
+      </c>
+      <c r="Q8" s="53">
+        <v>1000</v>
+      </c>
+      <c r="R8" s="53">
+        <v>25421</v>
+      </c>
+      <c r="S8" s="53">
+        <v>10014</v>
+      </c>
+      <c r="T8" s="54">
+        <f t="shared" si="0"/>
+        <v>2.5385460355502296</v>
+      </c>
+    </row>
+    <row r="9" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="39">
         <v>4</v>
       </c>
-      <c r="C9" s="26">
+      <c r="C9" s="40">
         <v>4000</v>
       </c>
-      <c r="D9" s="26">
+      <c r="D9" s="40">
         <v>205870</v>
       </c>
-      <c r="E9" s="26" t="s">
+      <c r="E9" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="29">
+      <c r="F9" s="41">
         <v>0.42680000000000001</v>
       </c>
-      <c r="I9" s="28">
+      <c r="I9" s="27">
         <v>4</v>
       </c>
-      <c r="J9" s="26">
+      <c r="J9" s="25">
         <v>4000</v>
       </c>
-      <c r="K9" s="26">
+      <c r="K9" s="25">
         <v>41918</v>
       </c>
-      <c r="L9" s="26" t="s">
+      <c r="L9" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="M9" s="29">
+      <c r="M9" s="61">
         <v>0.22919999999999999</v>
       </c>
-    </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="P9" s="55">
+        <v>4</v>
+      </c>
+      <c r="Q9" s="56">
+        <v>4000</v>
+      </c>
+      <c r="R9" s="56">
+        <v>205870</v>
+      </c>
+      <c r="S9" s="56">
+        <v>41918</v>
+      </c>
+      <c r="T9" s="57">
+        <f t="shared" si="0"/>
+        <v>4.911255307982251</v>
+      </c>
+    </row>
+    <row r="10" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="5"/>
     </row>
-    <row r="13" spans="2:13" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B13" s="36" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" s="36"/>
+    <row r="13" spans="2:20" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B13" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="34"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
-      <c r="I13" s="36" t="s">
+      <c r="I13" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="J13" s="36"/>
+      <c r="J13" s="34"/>
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
     </row>
-    <row r="14" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -2447,8 +2456,15 @@
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
-    </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="P14" s="45" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q14" s="46"/>
+      <c r="R14" s="46"/>
+      <c r="S14" s="46"/>
+      <c r="T14" s="47"/>
+    </row>
+    <row r="15" spans="2:20" ht="30" x14ac:dyDescent="0.25">
       <c r="B15" s="14" t="s">
         <v>0</v>
       </c>
@@ -2479,8 +2495,23 @@
       <c r="M15" s="16" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="P15" s="48" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="49" t="s">
+        <v>3</v>
+      </c>
+      <c r="R15" s="50" t="s">
+        <v>43</v>
+      </c>
+      <c r="S15" s="50" t="s">
+        <v>44</v>
+      </c>
+      <c r="T15" s="51" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B16" s="17">
         <v>1</v>
       </c>
@@ -2511,8 +2542,24 @@
       <c r="M16" s="18">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P16" s="52">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="53">
+        <v>50</v>
+      </c>
+      <c r="R16" s="58">
+        <v>10050</v>
+      </c>
+      <c r="S16" s="58">
+        <v>827</v>
+      </c>
+      <c r="T16" s="54">
+        <f>R16/S16</f>
+        <v>12.15235792019347</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B17" s="17">
         <v>2</v>
       </c>
@@ -2525,7 +2572,7 @@
       <c r="E17" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="F17" s="23">
+      <c r="F17" s="22">
         <v>0.28199999999999997</v>
       </c>
       <c r="I17" s="17">
@@ -2543,8 +2590,24 @@
       <c r="M17" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P17" s="52">
+        <v>2</v>
+      </c>
+      <c r="Q17" s="53">
+        <v>500</v>
+      </c>
+      <c r="R17" s="58">
+        <v>54830</v>
+      </c>
+      <c r="S17" s="58">
+        <v>6548</v>
+      </c>
+      <c r="T17" s="54">
+        <f t="shared" ref="T17:T19" si="1">R17/S17</f>
+        <v>8.3735491753207079</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B18" s="17">
         <v>3</v>
       </c>
@@ -2557,7 +2620,7 @@
       <c r="E18" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="22">
+      <c r="F18" s="21">
         <v>0.36599999999999999</v>
       </c>
       <c r="I18" s="17">
@@ -2575,40 +2638,72 @@
       <c r="M18" s="11">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="24">
+      <c r="P18" s="52">
+        <v>3</v>
+      </c>
+      <c r="Q18" s="53">
+        <v>1000</v>
+      </c>
+      <c r="R18" s="58">
+        <v>84013</v>
+      </c>
+      <c r="S18" s="58">
+        <v>17994</v>
+      </c>
+      <c r="T18" s="54">
+        <f t="shared" si="1"/>
+        <v>4.6689452039568744</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="23">
         <v>4</v>
       </c>
-      <c r="C19" s="25">
+      <c r="C19" s="24">
         <v>4000</v>
       </c>
-      <c r="D19" s="26">
+      <c r="D19" s="25">
         <v>307650</v>
       </c>
-      <c r="E19" s="26" t="s">
+      <c r="E19" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="F19" s="30">
+      <c r="F19" s="28">
         <v>0.40400000000000003</v>
       </c>
-      <c r="I19" s="24">
+      <c r="I19" s="23">
         <v>4</v>
       </c>
-      <c r="J19" s="25">
+      <c r="J19" s="24">
         <v>4000</v>
       </c>
-      <c r="K19" s="26">
+      <c r="K19" s="25">
         <v>61630</v>
       </c>
-      <c r="L19" s="26" t="s">
+      <c r="L19" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="M19" s="30">
+      <c r="M19" s="59">
         <v>0.34849999999999998</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="P19" s="55">
+        <v>4</v>
+      </c>
+      <c r="Q19" s="56">
+        <v>4000</v>
+      </c>
+      <c r="R19" s="40">
+        <v>307650</v>
+      </c>
+      <c r="S19" s="40">
+        <v>61630</v>
+      </c>
+      <c r="T19" s="57">
+        <f t="shared" si="1"/>
+        <v>4.9918870679863705</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
@@ -2616,42 +2711,42 @@
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B21" s="4"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
       <c r="F21" s="5"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B22" s="4"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="5"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B23" s="4"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="5"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B24" s="4"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="5"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B25" s="4"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="5"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
@@ -2659,7 +2754,7 @@
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -2669,7 +2764,7 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -2679,7 +2774,7 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -2689,7 +2784,7 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -2699,7 +2794,7 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -2739,8 +2834,341 @@
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
+    <row r="44" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C44" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="D44" s="34"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+    </row>
+    <row r="45" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C46" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="D46" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="E46" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="F46" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="G46" s="16" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C47" s="17">
+        <v>1</v>
+      </c>
+      <c r="D47" s="6">
+        <v>5</v>
+      </c>
+      <c r="E47" s="6">
+        <v>524</v>
+      </c>
+      <c r="F47" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G47" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C48" s="17">
+        <v>2</v>
+      </c>
+      <c r="D48" s="6">
+        <v>30</v>
+      </c>
+      <c r="E48" s="6">
+        <v>3163</v>
+      </c>
+      <c r="F48" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G48" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C49" s="17">
+        <v>3</v>
+      </c>
+      <c r="D49" s="6">
+        <v>50</v>
+      </c>
+      <c r="E49" s="6">
+        <v>8537</v>
+      </c>
+      <c r="F49" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G49" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C50" s="17">
+        <v>4</v>
+      </c>
+      <c r="D50" s="6">
+        <v>80</v>
+      </c>
+      <c r="E50" s="6">
+        <v>13767</v>
+      </c>
+      <c r="F50" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G50" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C51" s="17">
+        <v>5</v>
+      </c>
+      <c r="D51" s="6">
+        <v>200</v>
+      </c>
+      <c r="E51" s="6">
+        <v>35355</v>
+      </c>
+      <c r="F51" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G51" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C52" s="32">
+        <v>6</v>
+      </c>
+      <c r="D52" s="12">
+        <v>400</v>
+      </c>
+      <c r="E52" s="12">
+        <v>46017</v>
+      </c>
+      <c r="F52" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G52" s="33">
+        <v>0.20749999999999999</v>
+      </c>
+    </row>
+    <row r="53" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2"/>
+      <c r="G53" s="2"/>
+    </row>
+    <row r="54" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C54" s="3"/>
+      <c r="D54" s="3"/>
+      <c r="E54" s="3"/>
+      <c r="F54" s="3"/>
+      <c r="G54" s="5"/>
+    </row>
+    <row r="55" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C55" s="3"/>
+      <c r="D55" s="3"/>
+      <c r="E55" s="3"/>
+      <c r="F55" s="3"/>
+      <c r="G55" s="5"/>
+    </row>
+    <row r="56" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
+      <c r="E56" s="3"/>
+      <c r="F56" s="3"/>
+      <c r="G56" s="5"/>
+    </row>
+    <row r="57" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C57" s="2"/>
+      <c r="D57" s="2"/>
+      <c r="E57" s="2"/>
+      <c r="F57" s="2"/>
+      <c r="G57" s="2"/>
+    </row>
+    <row r="58" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C58" s="2"/>
+      <c r="D58" s="2"/>
+      <c r="E58" s="2"/>
+      <c r="F58" s="2"/>
+      <c r="G58" s="2"/>
+    </row>
+    <row r="59" spans="3:7" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C59" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="D59" s="34"/>
+      <c r="E59" s="2"/>
+      <c r="F59" s="2"/>
+      <c r="G59" s="2"/>
+    </row>
+    <row r="60" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C60" s="2"/>
+      <c r="D60" s="2"/>
+      <c r="E60" s="2"/>
+      <c r="F60" s="2"/>
+      <c r="G60" s="2"/>
+    </row>
+    <row r="61" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C61" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="D61" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="E61" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="F61" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="G61" s="16" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C62" s="17">
+        <v>1</v>
+      </c>
+      <c r="D62" s="6">
+        <v>5</v>
+      </c>
+      <c r="E62" s="6">
+        <v>1612</v>
+      </c>
+      <c r="F62" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G62" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C63" s="17">
+        <v>2</v>
+      </c>
+      <c r="D63" s="6">
+        <v>30</v>
+      </c>
+      <c r="E63" s="6">
+        <v>7175</v>
+      </c>
+      <c r="F63" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G63" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C64" s="17">
+        <v>3</v>
+      </c>
+      <c r="D64" s="6">
+        <v>50</v>
+      </c>
+      <c r="E64" s="6">
+        <v>8988</v>
+      </c>
+      <c r="F64" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G64" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C65" s="17">
+        <v>4</v>
+      </c>
+      <c r="D65" s="6">
+        <v>80</v>
+      </c>
+      <c r="E65" s="6">
+        <v>16977</v>
+      </c>
+      <c r="F65" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G65" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C66" s="17">
+        <v>5</v>
+      </c>
+      <c r="D66" s="6">
+        <v>200</v>
+      </c>
+      <c r="E66" s="6">
+        <v>20330</v>
+      </c>
+      <c r="F66" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G66" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C67" s="23">
+        <v>6</v>
+      </c>
+      <c r="D67" s="25">
+        <v>400</v>
+      </c>
+      <c r="E67" s="25">
+        <v>35200</v>
+      </c>
+      <c r="F67" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="G67" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C68" s="29">
+        <v>7</v>
+      </c>
+      <c r="D68" s="30">
+        <v>500</v>
+      </c>
+      <c r="E68" s="30">
+        <v>44977</v>
+      </c>
+      <c r="F68" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="G68" s="31">
+        <v>3.4000000000000002E-2</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="10">
+    <mergeCell ref="P4:T4"/>
+    <mergeCell ref="P14:T14"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="C59:D59"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="I3:J3"/>

</xml_diff>